<commit_message>
Chnage fixation location and more
- Take the first fixation break out of the loop instead of the last
- Fix number of blocks per run so it matches the excel file
- Fix sequence.mp3 to have 2 identical sequences
- Change the small screen init to match screen setup at home + comment out MRI params
</commit_message>
<xml_diff>
--- a/experiment timing.xlsx
+++ b/experiment timing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\code\auditory-motor-fMRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\MSc-neuroscience\auditory-experiment-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6D97AE-CE9A-49EE-B38B-72C8D66AEF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87131CFA-2CD2-48D4-9689-169D8A8A6224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{1F19B5B7-407E-4C05-84E6-D57B900D1867}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1F19B5B7-407E-4C05-84E6-D57B900D1867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -88,7 +85,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -97,7 +94,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -442,25 +439,26 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -468,7 +466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -476,7 +474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -484,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -492,15 +490,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -508,7 +506,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -517,21 +515,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14">
-        <f>B10*B13</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <f>B10*B13+B5</f>
+        <v>368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -539,7 +537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -547,7 +545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -555,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -563,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -571,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -580,13 +578,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27">
-        <f>B24*B26</f>
-        <v>52</v>
+        <f>B24*B26+B21</f>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>